<commit_message>
Atualização automática de FORO_REGIONAL_DA_TRISTEZA.xlsx
</commit_message>
<xml_diff>
--- a/FORO_REGIONAL_DA_TRISTEZA.xlsx
+++ b/FORO_REGIONAL_DA_TRISTEZA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98D6A5AE-6597-4273-AE5E-6B3FA627C27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D000500D-F229-4DD4-BB3C-434DBD1A96C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1147,7 +1147,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{12A08437-7DE5-4DDF-B6C0-6FE7E85EA838}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{5B463002-A09A-43AC-862A-64FA61122849}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1177,10 +1177,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93D02608-4B57-485B-BF62-E0E6A66C5B15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AAA0048-0D4B-4DB0-AF45-87B706FF6294}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1218,7 +1218,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD51247-5CE4-49DA-AF37-4991AC135775}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCBD577-4CE5-4277-9F9B-8874FCB89E15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,7 +1281,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B8E49F-E773-4DAB-946A-2F4F3FF84111}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC33FD5-7859-4138-9CAE-F1F13D52D054}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1300,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BC82928-95B8-F3A2-4B55-5CAB20107CC7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED3DFF8E-2DE0-3EA8-C7E2-ACC4F70F0CF8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1349,7 +1349,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68B3F952-72FE-6432-BB0B-9FADD998F977}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CC1E26C-978D-722C-4835-2F817AAF20B8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1368,7 +1368,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90F437B7-AB32-8104-C706-502EA05938E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D66F712-C05C-C7E2-03E7-8DADD3751D16}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1399,7 +1399,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6366135E-5564-E027-2AE6-B41FA0F8F131}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08005E07-168F-078F-F819-094FFC8BA7D4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1430,7 +1430,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1290E540-11C6-C9E2-841C-5DEC914E650B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5091EE92-5998-5DF7-56E2-42535F9C3DF2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1473,7 +1473,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3D92B7-7D25-4AD5-A7AE-003575723704}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E2B7503-BFEF-4773-AA51-07D71A12E6FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1511,7 +1511,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DD08ED-A45C-4AF3-B6EB-089137A00B91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F688B65-2BF5-4EFF-852D-6822A95C6484}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1554,7 +1554,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32CF7C29-6B60-4B7C-9000-4D6968909C1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9845852-5D98-4CAE-BA93-B8186077DE4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1867,7 +1867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EBE0AA-43F0-4124-9536-973C1055DF13}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6233C86E-9EB3-4598-B433-3DB8ACDE0DBC}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5114,16 +5114,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>